<commit_message>
chore: update the intent xlsx file.
</commit_message>
<xml_diff>
--- a/intents.xlsx
+++ b/intents.xlsx
@@ -20,30 +20,75 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
-  <si>
-    <t xml:space="preserve">invoice</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Of course! The invoice for your purchase will be sent along with your goods. You can also download an electronic version from your account</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Do you have an invoice</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Can i get an invoice</t>
-  </si>
-  <si>
-    <t xml:space="preserve">information</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Hello ! I can provide you with information about our payment and shipping policies.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">I have a question.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">I need some information ? </t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="23">
+  <si>
+    <t xml:space="preserve">Do you ship worldwide ?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Your purchase can be shipped worldwide. However, delivery charges may vary.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">What is your shipping policy ?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Do you ship to Europe ? </t>
+  </si>
+  <si>
+    <t xml:space="preserve">What are your accepted payment options?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">You can pay for your purchase with Visa, Mastercard or using a PayPal account.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Are Visa cards accepted ?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Can i use Mastercard to pay my purchase ?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Can i pay using PayPal? </t>
+  </si>
+  <si>
+    <t xml:space="preserve">I need assistance.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Please reach us at contact@my-sample-company.com for further assistance.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">I want a refund.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">I have a problem.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">I never received my purchase.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Can you send me an invoice?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The invoice for your purchase will be sent along with your goods. You can also download an electronic version from your account.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Hello</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Hello! I can provide you with information about our payment and shipping policies.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">What's up?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Good morning</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Hi</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Can I get an invoice ?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Of course! The invoice for your purchase will be sent along with your goods. You can also download an electronic version from your account.</t>
   </si>
 </sst>
 </file>
@@ -53,7 +98,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="5">
+  <fonts count="4">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -74,11 +119,6 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="0"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -128,7 +168,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -153,10 +193,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:C9"/>
+  <dimension ref="A1:C34"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A15" activeCellId="0" sqref="A15"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A18" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A34" activeCellId="0" sqref="A34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -189,24 +229,129 @@
         <v>3</v>
       </c>
     </row>
-    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="0" t="s">
-        <v>4</v>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="0" t="s">
+        <v>0</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="0" t="s">
         <v>7</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="0" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="0" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="0" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="0" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="0" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="0" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="0" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="0" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="0" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A22" s="0" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A23" s="0" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A25" s="0" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A26" s="0" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A27" s="0" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A28" s="0" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A29" s="0" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A30" s="0" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A32" s="0" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A33" s="0" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A34" s="0" t="s">
+        <v>21</v>
       </c>
     </row>
   </sheetData>

</xml_diff>